<commit_message>
Use ₱ sign for total amount
</commit_message>
<xml_diff>
--- a/src/assets/formats/short.xlsx
+++ b/src/assets/formats/short.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mac\Documents\GitHub\billing-client\src\assets\formats\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C38ADE3-CA19-42FE-BDFB-D54BDB44BB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6036FF-CC87-4F4B-993F-A9B991DEE765}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{45D3D4AD-488A-416E-B4D0-07C98B8D3610}"/>
   </bookViews>
@@ -99,8 +99,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="\P#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="\₱\ #,##0.00"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -370,12 +370,6 @@
     <xf numFmtId="4" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -454,8 +448,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -773,8 +773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20EDD0AB-27CF-4FAB-A7E6-83000BE6AA48}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="I49" sqref="I49:J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -790,198 +790,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
     </row>
     <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
     </row>
     <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
     </row>
     <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
     </row>
     <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
     </row>
     <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
+      <c r="B8" s="22"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
     </row>
     <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="45" t="s">
+      <c r="B10" s="41"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="H10" s="45"/>
-      <c r="I10" s="46"/>
-      <c r="J10" s="46"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
     </row>
     <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="34" t="s">
+      <c r="C13" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="36"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="39"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="40"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="42"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="40"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="22"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="21"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="26" t="s">
+      <c r="F18" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="28" t="s">
+      <c r="G18" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H18" s="29"/>
-      <c r="I18" s="28" t="s">
+      <c r="H18" s="27"/>
+      <c r="I18" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="J18" s="29"/>
+      <c r="J18" s="27"/>
     </row>
     <row r="19" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="25"/>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="27"/>
-      <c r="G19" s="30" t="s">
+      <c r="F19" s="25"/>
+      <c r="G19" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="H19" s="31"/>
-      <c r="I19" s="30"/>
-      <c r="J19" s="31"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="29"/>
     </row>
     <row r="20" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
       <c r="D20" s="8"/>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -991,9 +991,9 @@
       <c r="J20" s="17"/>
     </row>
     <row r="21" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
+      <c r="A21" s="18"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="8"/>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1003,9 +1003,9 @@
       <c r="J21" s="17"/>
     </row>
     <row r="22" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
+      <c r="A22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="8"/>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1015,9 +1015,9 @@
       <c r="J22" s="17"/>
     </row>
     <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
+      <c r="A23" s="18"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="8"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1027,9 +1027,9 @@
       <c r="J23" s="17"/>
     </row>
     <row r="24" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
+      <c r="A24" s="18"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="8"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1039,9 +1039,9 @@
       <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="A25" s="18"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
       <c r="D25" s="8"/>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1051,9 +1051,9 @@
       <c r="J25" s="17"/>
     </row>
     <row r="26" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+      <c r="A26" s="18"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
       <c r="D26" s="8"/>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -1063,9 +1063,9 @@
       <c r="J26" s="17"/>
     </row>
     <row r="27" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
+      <c r="A27" s="18"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
       <c r="D27" s="8"/>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1075,9 +1075,9 @@
       <c r="J27" s="17"/>
     </row>
     <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
+      <c r="A28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="8"/>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1087,9 +1087,9 @@
       <c r="J28" s="17"/>
     </row>
     <row r="29" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="8"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -1099,9 +1099,9 @@
       <c r="J29" s="17"/>
     </row>
     <row r="30" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
+      <c r="A30" s="18"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="8"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1111,9 +1111,9 @@
       <c r="J30" s="17"/>
     </row>
     <row r="31" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="8"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1123,9 +1123,9 @@
       <c r="J31" s="17"/>
     </row>
     <row r="32" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
+      <c r="A32" s="18"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
       <c r="D32" s="8"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -1135,9 +1135,9 @@
       <c r="J32" s="17"/>
     </row>
     <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
+      <c r="A33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="8"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -1147,9 +1147,9 @@
       <c r="J33" s="17"/>
     </row>
     <row r="34" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
       <c r="D34" s="8"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -1159,9 +1159,9 @@
       <c r="J34" s="17"/>
     </row>
     <row r="35" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="20"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
+      <c r="A35" s="18"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="8"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -1171,9 +1171,9 @@
       <c r="J35" s="17"/>
     </row>
     <row r="36" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="21"/>
+      <c r="A36" s="18"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="8"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -1183,9 +1183,9 @@
       <c r="J36" s="17"/>
     </row>
     <row r="37" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="21"/>
+      <c r="A37" s="18"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="8"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -1195,9 +1195,9 @@
       <c r="J37" s="17"/>
     </row>
     <row r="38" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="21"/>
+      <c r="A38" s="18"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="8"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -1207,9 +1207,9 @@
       <c r="J38" s="17"/>
     </row>
     <row r="39" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="21"/>
+      <c r="A39" s="18"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="8"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -1219,9 +1219,9 @@
       <c r="J39" s="17"/>
     </row>
     <row r="40" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="21"/>
+      <c r="A40" s="18"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
       <c r="D40" s="8"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -1231,9 +1231,9 @@
       <c r="J40" s="17"/>
     </row>
     <row r="41" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="20"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="21"/>
+      <c r="A41" s="18"/>
+      <c r="B41" s="19"/>
+      <c r="C41" s="19"/>
       <c r="D41" s="8"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1243,9 +1243,9 @@
       <c r="J41" s="17"/>
     </row>
     <row r="42" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="20"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="21"/>
+      <c r="A42" s="18"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="8"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -1255,9 +1255,9 @@
       <c r="J42" s="17"/>
     </row>
     <row r="43" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="20"/>
-      <c r="B43" s="21"/>
-      <c r="C43" s="21"/>
+      <c r="A43" s="18"/>
+      <c r="B43" s="19"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="8"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -1267,9 +1267,9 @@
       <c r="J43" s="17"/>
     </row>
     <row r="44" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="21"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="8"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -1279,9 +1279,9 @@
       <c r="J44" s="17"/>
     </row>
     <row r="45" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="20"/>
-      <c r="B45" s="21"/>
-      <c r="C45" s="21"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="8"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -1291,9 +1291,9 @@
       <c r="J45" s="17"/>
     </row>
     <row r="46" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="20"/>
-      <c r="B46" s="21"/>
-      <c r="C46" s="21"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="19"/>
       <c r="D46" s="8"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -1303,9 +1303,9 @@
       <c r="J46" s="17"/>
     </row>
     <row r="47" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="20"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
       <c r="D47" s="8"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -1315,9 +1315,9 @@
       <c r="J47" s="17"/>
     </row>
     <row r="48" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="20"/>
-      <c r="B48" s="21"/>
-      <c r="C48" s="21"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="8"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -1337,8 +1337,8 @@
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="11"/>
-      <c r="I49" s="18"/>
-      <c r="J49" s="19"/>
+      <c r="I49" s="45"/>
+      <c r="J49" s="46"/>
     </row>
     <row r="50" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="13"/>

</xml_diff>